<commit_message>
Commit atualizacao tesouro 03/07
</commit_message>
<xml_diff>
--- a/TITULO COMPRADO - LIVIO - 0719.xlsx
+++ b/TITULO COMPRADO - LIVIO - 0719.xlsx
@@ -627,6 +627,9 @@
                   <c:pt idx="1">
                     <c:v>02/07</c:v>
                   </c:pt>
+                  <c:pt idx="2">
+                    <c:v>03/07</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -717,6 +720,9 @@
                 </c:pt>
                 <c:pt idx="1" formatCode="General">
                   <c:v>3.71</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="General">
+                  <c:v>3.76</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -780,6 +786,9 @@
                   <c:pt idx="1">
                     <c:v>02/07</c:v>
                   </c:pt>
+                  <c:pt idx="2">
+                    <c:v>03/07</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -871,6 +880,9 @@
                 <c:pt idx="1" formatCode="General">
                   <c:v>3.59</c:v>
                 </c:pt>
+                <c:pt idx="2" formatCode="General">
+                  <c:v>3.64</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -886,8 +898,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="627773984"/>
-        <c:axId val="627778880"/>
+        <c:axId val="915655248"/>
+        <c:axId val="1190381424"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -955,6 +967,9 @@
                         </c:pt>
                         <c:pt idx="1">
                           <c:v>02/07</c:v>
+                        </c:pt>
+                        <c:pt idx="2">
+                          <c:v>03/07</c:v>
                         </c:pt>
                       </c:lvl>
                       <c:lvl>
@@ -1181,6 +1196,9 @@
                         <c:pt idx="1">
                           <c:v>02/07</c:v>
                         </c:pt>
+                        <c:pt idx="2">
+                          <c:v>03/07</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -1344,7 +1362,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="627773984"/>
+        <c:axId val="915655248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1387,7 +1405,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="627778880"/>
+        <c:crossAx val="1190381424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1395,7 +1413,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="627778880"/>
+        <c:axId val="1190381424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1446,7 +1464,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="627773984"/>
+        <c:crossAx val="915655248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1665,6 +1683,9 @@
                   <c:pt idx="1">
                     <c:v>02/07</c:v>
                   </c:pt>
+                  <c:pt idx="2">
+                    <c:v>03/07</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -1755,6 +1776,9 @@
                 </c:pt>
                 <c:pt idx="1" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>1814.5</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                  <c:v>1800.97</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1818,6 +1842,9 @@
                   <c:pt idx="1">
                     <c:v>02/07</c:v>
                   </c:pt>
+                  <c:pt idx="2">
+                    <c:v>03/07</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -1909,6 +1936,9 @@
                 <c:pt idx="1" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>1848.04</c:v>
                 </c:pt>
+                <c:pt idx="2" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                  <c:v>1834.23</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1924,11 +1954,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="627776160"/>
-        <c:axId val="627777248"/>
+        <c:axId val="1190377072"/>
+        <c:axId val="1190374896"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="627776160"/>
+        <c:axId val="1190377072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1971,7 +2001,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="627777248"/>
+        <c:crossAx val="1190374896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1979,7 +2009,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="627777248"/>
+        <c:axId val="1190374896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2030,7 +2060,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="627776160"/>
+        <c:crossAx val="1190377072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2219,6 +2249,9 @@
                   <c:pt idx="1">
                     <c:v>02/07</c:v>
                   </c:pt>
+                  <c:pt idx="2">
+                    <c:v>03/07</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -2432,6 +2465,9 @@
                   <c:pt idx="1">
                     <c:v>02/07</c:v>
                   </c:pt>
+                  <c:pt idx="2">
+                    <c:v>03/07</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -2598,8 +2634,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="586007680"/>
-        <c:axId val="586015296"/>
+        <c:axId val="1190378704"/>
+        <c:axId val="1190372720"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -2668,6 +2704,9 @@
                         <c:pt idx="1">
                           <c:v>02/07</c:v>
                         </c:pt>
+                        <c:pt idx="2">
+                          <c:v>03/07</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -2760,6 +2799,9 @@
                       </c:pt>
                       <c:pt idx="1" formatCode="General">
                         <c:v>3.71</c:v>
+                      </c:pt>
+                      <c:pt idx="2" formatCode="General">
+                        <c:v>3.76</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2833,6 +2875,9 @@
                         <c:pt idx="1">
                           <c:v>02/07</c:v>
                         </c:pt>
+                        <c:pt idx="2">
+                          <c:v>03/07</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -2926,6 +2971,9 @@
                       <c:pt idx="1" formatCode="General">
                         <c:v>3.59</c:v>
                       </c:pt>
+                      <c:pt idx="2" formatCode="General">
+                        <c:v>3.64</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -2936,7 +2984,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="586007680"/>
+        <c:axId val="1190378704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2979,7 +3027,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="586015296"/>
+        <c:crossAx val="1190372720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2987,7 +3035,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="586015296"/>
+        <c:axId val="1190372720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3038,7 +3086,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="586007680"/>
+        <c:crossAx val="1190378704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3226,6 +3274,9 @@
                   <c:pt idx="1">
                     <c:v>02/07</c:v>
                   </c:pt>
+                  <c:pt idx="2">
+                    <c:v>03/07</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -3439,6 +3490,9 @@
                   <c:pt idx="1">
                     <c:v>02/07</c:v>
                   </c:pt>
+                  <c:pt idx="2">
+                    <c:v>03/07</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -3605,8 +3659,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="586009856"/>
-        <c:axId val="414433344"/>
+        <c:axId val="1190385232"/>
+        <c:axId val="1190371632"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -3675,6 +3729,9 @@
                         <c:pt idx="1">
                           <c:v>02/07</c:v>
                         </c:pt>
+                        <c:pt idx="2">
+                          <c:v>03/07</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -3767,6 +3824,9 @@
                       </c:pt>
                       <c:pt idx="1" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>1814.5</c:v>
+                      </c:pt>
+                      <c:pt idx="2" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1800.97</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -3840,6 +3900,9 @@
                         <c:pt idx="1">
                           <c:v>02/07</c:v>
                         </c:pt>
+                        <c:pt idx="2">
+                          <c:v>03/07</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -3933,6 +3996,9 @@
                       <c:pt idx="1" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>1848.04</c:v>
                       </c:pt>
+                      <c:pt idx="2" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1834.23</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -3943,7 +4009,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="586009856"/>
+        <c:axId val="1190385232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3986,7 +4052,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="414433344"/>
+        <c:crossAx val="1190371632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3994,7 +4060,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="414433344"/>
+        <c:axId val="1190371632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4045,7 +4111,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="586009856"/>
+        <c:crossAx val="1190385232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7073,7 +7139,7 @@
   <dimension ref="A2:DO11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AV6" sqref="AV6"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7357,8 +7423,12 @@
       <c r="G3" s="53">
         <v>43648</v>
       </c>
-      <c r="H3" s="55"/>
-      <c r="I3" s="55"/>
+      <c r="H3" s="55">
+        <v>43649</v>
+      </c>
+      <c r="I3" s="55">
+        <v>43649</v>
+      </c>
       <c r="J3" s="20"/>
       <c r="K3" s="21"/>
       <c r="L3" s="22"/>
@@ -7492,8 +7562,12 @@
       <c r="G4" s="57">
         <v>1814.5</v>
       </c>
-      <c r="H4" s="31"/>
-      <c r="I4" s="32"/>
+      <c r="H4" s="31">
+        <v>3.76</v>
+      </c>
+      <c r="I4" s="32">
+        <v>1800.97</v>
+      </c>
       <c r="J4" s="31"/>
       <c r="K4" s="32"/>
       <c r="L4" s="31"/>
@@ -7627,8 +7701,12 @@
       <c r="G5" s="15">
         <v>1848.04</v>
       </c>
-      <c r="H5" s="42"/>
-      <c r="I5" s="43"/>
+      <c r="H5" s="42">
+        <v>3.64</v>
+      </c>
+      <c r="I5" s="43">
+        <v>1834.23</v>
+      </c>
       <c r="J5" s="42"/>
       <c r="K5" s="43"/>
       <c r="L5" s="42"/>

</xml_diff>

<commit_message>
Commit atualizacao tesouro 04/07
</commit_message>
<xml_diff>
--- a/TITULO COMPRADO - LIVIO - 0719.xlsx
+++ b/TITULO COMPRADO - LIVIO - 0719.xlsx
@@ -630,6 +630,9 @@
                   <c:pt idx="2">
                     <c:v>03/07</c:v>
                   </c:pt>
+                  <c:pt idx="3">
+                    <c:v>04/07</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -723,6 +726,9 @@
                 </c:pt>
                 <c:pt idx="2" formatCode="General">
                   <c:v>3.76</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>3.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -789,6 +795,9 @@
                   <c:pt idx="2">
                     <c:v>03/07</c:v>
                   </c:pt>
+                  <c:pt idx="3">
+                    <c:v>04/07</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -883,6 +892,9 @@
                 <c:pt idx="2" formatCode="General">
                   <c:v>3.64</c:v>
                 </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>3.58</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -898,8 +910,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="915655248"/>
-        <c:axId val="1190381424"/>
+        <c:axId val="1343501760"/>
+        <c:axId val="1429731552"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -970,6 +982,9 @@
                         </c:pt>
                         <c:pt idx="2">
                           <c:v>03/07</c:v>
+                        </c:pt>
+                        <c:pt idx="3">
+                          <c:v>04/07</c:v>
                         </c:pt>
                       </c:lvl>
                       <c:lvl>
@@ -1199,6 +1214,9 @@
                         <c:pt idx="2">
                           <c:v>03/07</c:v>
                         </c:pt>
+                        <c:pt idx="3">
+                          <c:v>04/07</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -1362,7 +1380,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="915655248"/>
+        <c:axId val="1343501760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1405,7 +1423,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1190381424"/>
+        <c:crossAx val="1429731552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1413,7 +1431,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1190381424"/>
+        <c:axId val="1429731552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1464,7 +1482,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="915655248"/>
+        <c:crossAx val="1343501760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1686,6 +1704,9 @@
                   <c:pt idx="2">
                     <c:v>03/07</c:v>
                   </c:pt>
+                  <c:pt idx="3">
+                    <c:v>04/07</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -1779,6 +1800,9 @@
                 </c:pt>
                 <c:pt idx="2" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>1800.97</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                  <c:v>1817.76</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1845,6 +1869,9 @@
                   <c:pt idx="2">
                     <c:v>03/07</c:v>
                   </c:pt>
+                  <c:pt idx="3">
+                    <c:v>04/07</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -1939,6 +1966,9 @@
                 <c:pt idx="2" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>1834.23</c:v>
                 </c:pt>
+                <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                  <c:v>1851.34</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1954,11 +1984,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1190377072"/>
-        <c:axId val="1190374896"/>
+        <c:axId val="1429729920"/>
+        <c:axId val="1429735904"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1190377072"/>
+        <c:axId val="1429729920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2001,7 +2031,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1190374896"/>
+        <c:crossAx val="1429735904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2009,7 +2039,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1190374896"/>
+        <c:axId val="1429735904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2060,7 +2090,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1190377072"/>
+        <c:crossAx val="1429729920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2252,6 +2282,9 @@
                   <c:pt idx="2">
                     <c:v>03/07</c:v>
                   </c:pt>
+                  <c:pt idx="3">
+                    <c:v>04/07</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -2468,6 +2501,9 @@
                   <c:pt idx="2">
                     <c:v>03/07</c:v>
                   </c:pt>
+                  <c:pt idx="3">
+                    <c:v>04/07</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -2634,8 +2670,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1190378704"/>
-        <c:axId val="1190372720"/>
+        <c:axId val="1429730464"/>
+        <c:axId val="1429729376"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -2707,6 +2743,9 @@
                         <c:pt idx="2">
                           <c:v>03/07</c:v>
                         </c:pt>
+                        <c:pt idx="3">
+                          <c:v>04/07</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -2802,6 +2841,9 @@
                       </c:pt>
                       <c:pt idx="2" formatCode="General">
                         <c:v>3.76</c:v>
+                      </c:pt>
+                      <c:pt idx="3" formatCode="General">
+                        <c:v>3.7</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2878,6 +2920,9 @@
                         <c:pt idx="2">
                           <c:v>03/07</c:v>
                         </c:pt>
+                        <c:pt idx="3">
+                          <c:v>04/07</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -2974,6 +3019,9 @@
                       <c:pt idx="2" formatCode="General">
                         <c:v>3.64</c:v>
                       </c:pt>
+                      <c:pt idx="3" formatCode="General">
+                        <c:v>3.58</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -2984,7 +3032,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1190378704"/>
+        <c:axId val="1429730464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3027,7 +3075,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1190372720"/>
+        <c:crossAx val="1429729376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3035,7 +3083,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1190372720"/>
+        <c:axId val="1429729376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3086,7 +3134,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1190378704"/>
+        <c:crossAx val="1429730464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3277,6 +3325,9 @@
                   <c:pt idx="2">
                     <c:v>03/07</c:v>
                   </c:pt>
+                  <c:pt idx="3">
+                    <c:v>04/07</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -3493,6 +3544,9 @@
                   <c:pt idx="2">
                     <c:v>03/07</c:v>
                   </c:pt>
+                  <c:pt idx="3">
+                    <c:v>04/07</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -3659,8 +3713,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1190385232"/>
-        <c:axId val="1190371632"/>
+        <c:axId val="1429732096"/>
+        <c:axId val="1429743520"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -3732,6 +3786,9 @@
                         <c:pt idx="2">
                           <c:v>03/07</c:v>
                         </c:pt>
+                        <c:pt idx="3">
+                          <c:v>04/07</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -3827,6 +3884,9 @@
                       </c:pt>
                       <c:pt idx="2" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>1800.97</c:v>
+                      </c:pt>
+                      <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1817.76</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -3903,6 +3963,9 @@
                         <c:pt idx="2">
                           <c:v>03/07</c:v>
                         </c:pt>
+                        <c:pt idx="3">
+                          <c:v>04/07</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -3999,6 +4062,9 @@
                       <c:pt idx="2" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>1834.23</c:v>
                       </c:pt>
+                      <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1851.34</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -4009,7 +4075,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1190385232"/>
+        <c:axId val="1429732096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4052,7 +4118,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1190371632"/>
+        <c:crossAx val="1429743520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4060,7 +4126,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1190371632"/>
+        <c:axId val="1429743520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4111,7 +4177,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1190385232"/>
+        <c:crossAx val="1429732096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7138,8 +7204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:DO11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7429,8 +7495,12 @@
       <c r="I3" s="55">
         <v>43649</v>
       </c>
-      <c r="J3" s="20"/>
-      <c r="K3" s="21"/>
+      <c r="J3" s="20">
+        <v>43650</v>
+      </c>
+      <c r="K3" s="21">
+        <v>43650</v>
+      </c>
       <c r="L3" s="22"/>
       <c r="M3" s="23"/>
       <c r="N3" s="22"/>
@@ -7568,8 +7638,12 @@
       <c r="I4" s="32">
         <v>1800.97</v>
       </c>
-      <c r="J4" s="31"/>
-      <c r="K4" s="32"/>
+      <c r="J4" s="31">
+        <v>3.7</v>
+      </c>
+      <c r="K4" s="32">
+        <v>1817.76</v>
+      </c>
       <c r="L4" s="31"/>
       <c r="M4" s="32"/>
       <c r="N4" s="31"/>
@@ -7707,8 +7781,12 @@
       <c r="I5" s="43">
         <v>1834.23</v>
       </c>
-      <c r="J5" s="42"/>
-      <c r="K5" s="43"/>
+      <c r="J5" s="42">
+        <v>3.58</v>
+      </c>
+      <c r="K5" s="43">
+        <v>1851.34</v>
+      </c>
       <c r="L5" s="42"/>
       <c r="M5" s="15"/>
       <c r="N5" s="42"/>

</xml_diff>

<commit_message>
Commit atualizacao tesouro 08/07
</commit_message>
<xml_diff>
--- a/TITULO COMPRADO - LIVIO - 0719.xlsx
+++ b/TITULO COMPRADO - LIVIO - 0719.xlsx
@@ -534,7 +534,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -633,6 +632,12 @@
                   <c:pt idx="3">
                     <c:v>04/07</c:v>
                   </c:pt>
+                  <c:pt idx="4">
+                    <c:v>05/jul</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>08/jul</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -729,6 +734,12 @@
                 </c:pt>
                 <c:pt idx="3" formatCode="General">
                   <c:v>3.7</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>3.76</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>3.73</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -798,6 +809,12 @@
                   <c:pt idx="3">
                     <c:v>04/07</c:v>
                   </c:pt>
+                  <c:pt idx="4">
+                    <c:v>05/jul</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>08/jul</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -895,6 +912,12 @@
                 <c:pt idx="3" formatCode="General">
                   <c:v>3.58</c:v>
                 </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>3.64</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>3.61</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -910,8 +933,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1343501760"/>
-        <c:axId val="1429731552"/>
+        <c:axId val="1055270304"/>
+        <c:axId val="1055274112"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -985,6 +1008,12 @@
                         </c:pt>
                         <c:pt idx="3">
                           <c:v>04/07</c:v>
+                        </c:pt>
+                        <c:pt idx="4">
+                          <c:v>05/jul</c:v>
+                        </c:pt>
+                        <c:pt idx="5">
+                          <c:v>08/jul</c:v>
                         </c:pt>
                       </c:lvl>
                       <c:lvl>
@@ -1217,6 +1246,12 @@
                         <c:pt idx="3">
                           <c:v>04/07</c:v>
                         </c:pt>
+                        <c:pt idx="4">
+                          <c:v>05/jul</c:v>
+                        </c:pt>
+                        <c:pt idx="5">
+                          <c:v>08/jul</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -1380,7 +1415,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1343501760"/>
+        <c:axId val="1055270304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1423,7 +1458,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1429731552"/>
+        <c:crossAx val="1055274112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1431,7 +1466,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1429731552"/>
+        <c:axId val="1055274112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1482,7 +1517,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1343501760"/>
+        <c:crossAx val="1055270304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1496,7 +1531,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1608,7 +1642,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1707,6 +1740,12 @@
                   <c:pt idx="3">
                     <c:v>04/07</c:v>
                   </c:pt>
+                  <c:pt idx="4">
+                    <c:v>05/jul</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>08/jul</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -1803,6 +1842,12 @@
                 </c:pt>
                 <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>1817.76</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                  <c:v>1801.42</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                  <c:v>1810.17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1872,6 +1917,12 @@
                   <c:pt idx="3">
                     <c:v>04/07</c:v>
                   </c:pt>
+                  <c:pt idx="4">
+                    <c:v>05/jul</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>08/jul</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -1969,6 +2020,12 @@
                 <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>1851.34</c:v>
                 </c:pt>
+                <c:pt idx="4" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                  <c:v>1834.68</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                  <c:v>1843.57</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1984,11 +2041,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1429729920"/>
-        <c:axId val="1429735904"/>
+        <c:axId val="1055278464"/>
+        <c:axId val="1055274656"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1429729920"/>
+        <c:axId val="1055278464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2031,7 +2088,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1429735904"/>
+        <c:crossAx val="1055274656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2039,7 +2096,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1429735904"/>
+        <c:axId val="1055274656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2090,7 +2147,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1429729920"/>
+        <c:crossAx val="1055278464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2104,7 +2161,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2285,6 +2341,12 @@
                   <c:pt idx="3">
                     <c:v>04/07</c:v>
                   </c:pt>
+                  <c:pt idx="4">
+                    <c:v>05/jul</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>08/jul</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -2504,6 +2566,12 @@
                   <c:pt idx="3">
                     <c:v>04/07</c:v>
                   </c:pt>
+                  <c:pt idx="4">
+                    <c:v>05/jul</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>08/jul</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -2670,8 +2738,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1429730464"/>
-        <c:axId val="1429729376"/>
+        <c:axId val="1055270848"/>
+        <c:axId val="1055271392"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -2746,6 +2814,12 @@
                         <c:pt idx="3">
                           <c:v>04/07</c:v>
                         </c:pt>
+                        <c:pt idx="4">
+                          <c:v>05/jul</c:v>
+                        </c:pt>
+                        <c:pt idx="5">
+                          <c:v>08/jul</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -2844,6 +2918,12 @@
                       </c:pt>
                       <c:pt idx="3" formatCode="General">
                         <c:v>3.7</c:v>
+                      </c:pt>
+                      <c:pt idx="4" formatCode="General">
+                        <c:v>3.76</c:v>
+                      </c:pt>
+                      <c:pt idx="5" formatCode="General">
+                        <c:v>3.73</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2923,6 +3003,12 @@
                         <c:pt idx="3">
                           <c:v>04/07</c:v>
                         </c:pt>
+                        <c:pt idx="4">
+                          <c:v>05/jul</c:v>
+                        </c:pt>
+                        <c:pt idx="5">
+                          <c:v>08/jul</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -3022,6 +3108,12 @@
                       <c:pt idx="3" formatCode="General">
                         <c:v>3.58</c:v>
                       </c:pt>
+                      <c:pt idx="4" formatCode="General">
+                        <c:v>3.64</c:v>
+                      </c:pt>
+                      <c:pt idx="5" formatCode="General">
+                        <c:v>3.61</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -3032,7 +3124,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1429730464"/>
+        <c:axId val="1055270848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3075,7 +3167,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1429729376"/>
+        <c:crossAx val="1055271392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3083,7 +3175,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1429729376"/>
+        <c:axId val="1055271392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3134,7 +3226,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1429730464"/>
+        <c:crossAx val="1055270848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3328,6 +3420,12 @@
                   <c:pt idx="3">
                     <c:v>04/07</c:v>
                   </c:pt>
+                  <c:pt idx="4">
+                    <c:v>05/jul</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>08/jul</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -3547,6 +3645,12 @@
                   <c:pt idx="3">
                     <c:v>04/07</c:v>
                   </c:pt>
+                  <c:pt idx="4">
+                    <c:v>05/jul</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>08/jul</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -3713,8 +3817,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1429732096"/>
-        <c:axId val="1429743520"/>
+        <c:axId val="1055280640"/>
+        <c:axId val="1055281728"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -3789,6 +3893,12 @@
                         <c:pt idx="3">
                           <c:v>04/07</c:v>
                         </c:pt>
+                        <c:pt idx="4">
+                          <c:v>05/jul</c:v>
+                        </c:pt>
+                        <c:pt idx="5">
+                          <c:v>08/jul</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -3887,6 +3997,12 @@
                       </c:pt>
                       <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>1817.76</c:v>
+                      </c:pt>
+                      <c:pt idx="4" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1801.42</c:v>
+                      </c:pt>
+                      <c:pt idx="5" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1810.17</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -3966,6 +4082,12 @@
                         <c:pt idx="3">
                           <c:v>04/07</c:v>
                         </c:pt>
+                        <c:pt idx="4">
+                          <c:v>05/jul</c:v>
+                        </c:pt>
+                        <c:pt idx="5">
+                          <c:v>08/jul</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -4065,6 +4187,12 @@
                       <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>1851.34</c:v>
                       </c:pt>
+                      <c:pt idx="4" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1834.68</c:v>
+                      </c:pt>
+                      <c:pt idx="5" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1843.57</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -4075,7 +4203,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1429732096"/>
+        <c:axId val="1055280640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4118,7 +4246,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1429743520"/>
+        <c:crossAx val="1055281728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4126,7 +4254,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1429743520"/>
+        <c:axId val="1055281728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4177,7 +4305,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1429732096"/>
+        <c:crossAx val="1055280640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7204,8 +7332,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:DO11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7501,10 +7629,18 @@
       <c r="K3" s="21">
         <v>43650</v>
       </c>
-      <c r="L3" s="22"/>
-      <c r="M3" s="23"/>
-      <c r="N3" s="22"/>
-      <c r="O3" s="23"/>
+      <c r="L3" s="22">
+        <v>43651</v>
+      </c>
+      <c r="M3" s="23">
+        <v>43651</v>
+      </c>
+      <c r="N3" s="22">
+        <v>43654</v>
+      </c>
+      <c r="O3" s="23">
+        <v>43654</v>
+      </c>
       <c r="P3" s="22"/>
       <c r="Q3" s="23"/>
       <c r="R3" s="22"/>
@@ -7644,10 +7780,18 @@
       <c r="K4" s="32">
         <v>1817.76</v>
       </c>
-      <c r="L4" s="31"/>
-      <c r="M4" s="32"/>
-      <c r="N4" s="31"/>
-      <c r="O4" s="32"/>
+      <c r="L4" s="31">
+        <v>3.76</v>
+      </c>
+      <c r="M4" s="32">
+        <v>1801.42</v>
+      </c>
+      <c r="N4" s="31">
+        <v>3.73</v>
+      </c>
+      <c r="O4" s="32">
+        <v>1810.17</v>
+      </c>
       <c r="P4" s="31"/>
       <c r="Q4" s="32"/>
       <c r="R4" s="31"/>
@@ -7787,10 +7931,18 @@
       <c r="K5" s="43">
         <v>1851.34</v>
       </c>
-      <c r="L5" s="42"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="42"/>
-      <c r="O5" s="15"/>
+      <c r="L5" s="42">
+        <v>3.64</v>
+      </c>
+      <c r="M5" s="43">
+        <v>1834.68</v>
+      </c>
+      <c r="N5" s="56">
+        <v>3.61</v>
+      </c>
+      <c r="O5" s="57">
+        <v>1843.57</v>
+      </c>
       <c r="P5" s="42"/>
       <c r="Q5" s="43"/>
       <c r="R5" s="42"/>

</xml_diff>